<commit_message>
Add another merge in a test document.
</commit_message>
<xml_diff>
--- a/pso-xlsx-core/src/test/resources/org/pageseeder/xlsx/core/sample2.xlsx
+++ b/pso-xlsx-core/src/test/resources/org/pageseeder/xlsx/core/sample2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allette\projects\gitlab\xlsx\pso-xlsx-core\src\test\resources\org\pageseeder\xlsx\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49417C45-A8EB-4808-A8B7-9930C3809DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C8F050-D60E-4DE9-8E46-A86CE05EEFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement 3 - Table 3" sheetId="4" r:id="rId1"/>
@@ -286,10 +286,10 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Gardiner, Katrina - Personal View" guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="1942" windowHeight="1042" activeSheetId="66"/>
+    <customWorkbookView name="MacLeay, Andrea - Personal View" guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="9" windowWidth="1936" windowHeight="1056" activeSheetId="62"/>
+    <customWorkbookView name="Ireland, Peter - Personal View" guid="{8A1CB61A-793E-4812-8741-E8528853CB5E}" mergeInterval="0" personalView="1" windowWidth="952" windowHeight="1020" activeSheetId="60"/>
     <customWorkbookView name="Purwono, Antony - Personal View" guid="{4E28AB2B-9926-4755-99E6-883815CD2322}" mergeInterval="0" personalView="1" maximized="1" xWindow="2869" yWindow="-11" windowWidth="2902" windowHeight="1582" activeSheetId="31" showComments="commIndAndComment"/>
-    <customWorkbookView name="Ireland, Peter - Personal View" guid="{8A1CB61A-793E-4812-8741-E8528853CB5E}" mergeInterval="0" personalView="1" windowWidth="952" windowHeight="1020" activeSheetId="60"/>
-    <customWorkbookView name="MacLeay, Andrea - Personal View" guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="9" windowWidth="1936" windowHeight="1056" activeSheetId="62"/>
-    <customWorkbookView name="Gardiner, Katrina - Personal View" guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="1942" windowHeight="1042" activeSheetId="66"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -926,9 +926,6 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="5" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="7" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1199,6 +1196,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="6" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="30">
@@ -1921,7 +1921,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,12 +1945,12 @@
       <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="147" t="s">
+      <c r="C2" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -2331,11 +2331,11 @@
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="149" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
+      <c r="B20" s="149"/>
+      <c r="C20" s="149"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -2383,7 +2383,7 @@
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="38" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="18">
@@ -2410,19 +2410,19 @@
       <c r="A24" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="144">
+      <c r="B24" s="143">
         <v>-93.9</v>
       </c>
-      <c r="C24" s="144">
+      <c r="C24" s="143">
         <v>-230</v>
       </c>
-      <c r="D24" s="144">
+      <c r="D24" s="143">
         <v>-123.8</v>
       </c>
-      <c r="E24" s="144">
+      <c r="E24" s="143">
         <v>-100.8</v>
       </c>
-      <c r="F24" s="144">
+      <c r="F24" s="143">
         <v>-56.2</v>
       </c>
       <c r="G24"/>
@@ -2431,22 +2431,22 @@
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="145">
+      <c r="B25" s="144">
         <v>5</v>
       </c>
-      <c r="C25" s="145">
+      <c r="C25" s="144">
         <v>3.7</v>
       </c>
-      <c r="D25" s="145">
+      <c r="D25" s="144">
         <v>3.8</v>
       </c>
-      <c r="E25" s="145">
+      <c r="E25" s="144">
         <v>4</v>
       </c>
-      <c r="F25" s="145">
+      <c r="F25" s="144">
         <v>4.3</v>
       </c>
       <c r="G25"/>
@@ -2456,29 +2456,30 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4E28AB2B-9926-4755-99E6-883815CD2322}">
+    <customSheetView guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}" showPageBreaks="1" printArea="1">
       <selection activeCell="F12" sqref="F12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{8A1CB61A-793E-4812-8741-E8528853CB5E}">
+    <customSheetView guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}">
       <selection activeCell="F12" sqref="F12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}">
+    <customSheetView guid="{8A1CB61A-793E-4812-8741-E8528853CB5E}">
       <selection activeCell="F12" sqref="F12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}" showPageBreaks="1" printArea="1">
+    <customSheetView guid="{4E28AB2B-9926-4755-99E6-883815CD2322}">
       <selection activeCell="F12" sqref="F12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -2495,8 +2496,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="71" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="71"/>
+    <col min="1" max="1" width="30.28515625" style="70" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="70"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2510,17 +2511,17 @@
     </row>
     <row r="2" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="75"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -2532,13 +2533,13 @@
       <c r="E3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="75" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2555,32 +2556,32 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="80"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="79"/>
     </row>
     <row r="6" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="84">
+      <c r="B6" s="83">
         <v>6054</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="84">
         <v>8351</v>
       </c>
-      <c r="D6" s="85">
+      <c r="D6" s="84">
         <v>4044</v>
       </c>
-      <c r="E6" s="85">
+      <c r="E6" s="84">
         <v>14912</v>
       </c>
-      <c r="F6" s="146">
+      <c r="F6" s="145">
         <v>33360</v>
       </c>
     </row>
@@ -2629,222 +2630,222 @@
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="48">
         <v>-11830</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C11" s="47">
         <v>-32815</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="47">
         <v>-10867</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="47">
         <v>11514</v>
       </c>
-      <c r="F11" s="86">
+      <c r="F11" s="85">
         <v>-43998</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="48">
         <v>147952</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="47">
         <v>21045</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="47">
         <v>11324</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="47">
         <v>8866</v>
       </c>
-      <c r="F12" s="86">
+      <c r="F12" s="85">
         <v>189187</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="88"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="87"/>
     </row>
     <row r="14" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B14" s="48">
         <v>-159782</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="47">
         <v>-53860</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="47">
         <v>-22191</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="47">
         <v>2648</v>
       </c>
-      <c r="F14" s="86">
+      <c r="F14" s="85">
         <v>-233185</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="89"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="90"/>
     </row>
     <row r="16" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B16" s="48">
         <v>-41004</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="47">
         <v>-54512</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="47">
         <v>-61329</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E16" s="47">
         <v>-76012</v>
       </c>
-      <c r="F16" s="92">
+      <c r="F16" s="91">
         <v>-232857</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="93">
+      <c r="B17" s="92">
         <v>18922</v>
       </c>
-      <c r="C17" s="92">
+      <c r="C17" s="91">
         <v>11981</v>
       </c>
-      <c r="D17" s="92">
+      <c r="D17" s="91">
         <v>8407</v>
       </c>
-      <c r="E17" s="92">
+      <c r="E17" s="91">
         <v>8475</v>
       </c>
-      <c r="F17" s="92">
+      <c r="F17" s="91">
         <v>47784</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="94"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
     </row>
     <row r="19" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="95">
+      <c r="B19" s="94">
         <v>-59926</v>
       </c>
-      <c r="C19" s="96">
+      <c r="C19" s="95">
         <v>-66493</v>
       </c>
-      <c r="D19" s="96">
+      <c r="D19" s="95">
         <v>-69736</v>
       </c>
-      <c r="E19" s="96">
+      <c r="E19" s="95">
         <v>-84486</v>
       </c>
-      <c r="F19" s="96">
+      <c r="F19" s="95">
         <v>-280642</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="97"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
     </row>
     <row r="21" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="99">
+      <c r="B21" s="98">
         <v>-213654</v>
       </c>
-      <c r="C21" s="100">
+      <c r="C21" s="99">
         <v>-112003</v>
       </c>
-      <c r="D21" s="100">
+      <c r="D21" s="99">
         <v>-87883</v>
       </c>
-      <c r="E21" s="100">
+      <c r="E21" s="99">
         <v>-66926</v>
       </c>
-      <c r="F21" s="100">
+      <c r="F21" s="99">
         <v>-480466</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="82">
+      <c r="B22" s="81">
         <v>-11</v>
       </c>
-      <c r="C22" s="83">
+      <c r="C22" s="82">
         <v>-5.6</v>
       </c>
-      <c r="D22" s="83">
+      <c r="D22" s="82">
         <v>-4.2</v>
       </c>
-      <c r="E22" s="83">
+      <c r="E22" s="82">
         <v>-3</v>
       </c>
-      <c r="F22" s="74"/>
+      <c r="F22" s="73"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4E28AB2B-9926-4755-99E6-883815CD2322}">
+    <customSheetView guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}">
+      <selection activeCell="E22" sqref="E22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}">
       <selection activeCell="I21" sqref="I21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{8A1CB61A-793E-4812-8741-E8528853CB5E}">
       <selection activeCell="D8" sqref="D8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}">
-      <selection activeCell="I21" sqref="I21"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}">
-      <selection activeCell="E22" sqref="E22"/>
+    <customSheetView guid="{4E28AB2B-9926-4755-99E6-883815CD2322}">
+      <selection activeCell="I21" sqref="I21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
     </customSheetView>
@@ -2870,15 +2871,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="109" customWidth="1"/>
-    <col min="2" max="4" width="9.28515625" style="109" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="109" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="109" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="109"/>
+    <col min="1" max="1" width="27.85546875" style="108" customWidth="1"/>
+    <col min="2" max="4" width="9.28515625" style="108" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="108" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="108" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="108"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="57" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="4"/>
@@ -2887,17 +2888,17 @@
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="68"/>
-      <c r="B2" s="148" t="s">
+      <c r="A2" s="67"/>
+      <c r="B2" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="69"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:10" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
@@ -2915,7 +2916,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="12" t="s">
         <v>30</v>
       </c>
@@ -2933,36 +2934,36 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="59" t="s">
         <v>65</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="117"/>
+      <c r="F5" s="116"/>
     </row>
     <row r="6" spans="1:10" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="46">
         <v>12144</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="46">
         <v>17828</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="46">
         <v>11606</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="118" t="s">
+      <c r="F6" s="117" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2975,236 +2976,236 @@
       <c r="D7" s="6">
         <v>0.5</v>
       </c>
-      <c r="E7" s="119"/>
+      <c r="E7" s="118"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-    </row>
-    <row r="8" spans="1:10" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="111"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+    </row>
+    <row r="8" spans="1:10" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>68</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="119"/>
+      <c r="E8" s="118"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-    </row>
-    <row r="9" spans="1:10" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="G8" s="111"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+    </row>
+    <row r="9" spans="1:10" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="119"/>
+      <c r="E9" s="118"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-    </row>
-    <row r="10" spans="1:10" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="111"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+    </row>
+    <row r="10" spans="1:10" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="119"/>
+      <c r="E10" s="118"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
-    </row>
-    <row r="11" spans="1:10" s="105" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="G10" s="111"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101"/>
+    </row>
+    <row r="11" spans="1:10" s="104" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="47">
         <v>-12301</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C11" s="47">
         <v>-32813</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="47">
         <v>-10567</v>
       </c>
-      <c r="E11" s="61">
+      <c r="E11" s="60">
         <v>11730</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="44">
         <v>-43951</v>
       </c>
-      <c r="G11" s="114"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="104"/>
-    </row>
-    <row r="12" spans="1:10" s="105" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="G11" s="113"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="103"/>
+    </row>
+    <row r="12" spans="1:10" s="104" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="47">
         <v>127289</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="47">
         <v>20883</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="47">
         <v>11435</v>
       </c>
-      <c r="E12" s="61">
+      <c r="E12" s="60">
         <v>9131</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="44">
         <v>168737</v>
       </c>
-      <c r="G12" s="114"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="104"/>
-    </row>
-    <row r="13" spans="1:10" s="105" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="113"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="103"/>
+    </row>
+    <row r="13" spans="1:10" s="104" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="121"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
-    </row>
-    <row r="14" spans="1:10" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="63" t="s">
+      <c r="B13" s="119"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+    </row>
+    <row r="14" spans="1:10" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="52">
+      <c r="B14" s="51">
         <v>-139590</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>-53696</v>
       </c>
-      <c r="D14" s="52">
+      <c r="D14" s="51">
         <v>-22001</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>2599</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="45">
         <v>-212688</v>
       </c>
-      <c r="G14" s="110"/>
-    </row>
-    <row r="15" spans="1:10" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="109"/>
+    </row>
+    <row r="15" spans="1:10" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="110"/>
-    </row>
-    <row r="16" spans="1:10" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="109"/>
+    </row>
+    <row r="16" spans="1:10" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="110"/>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107"/>
-    </row>
-    <row r="17" spans="1:9" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="64" t="s">
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="106"/>
+    </row>
+    <row r="17" spans="1:9" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="48">
+      <c r="B17" s="47">
         <v>-42524</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="47">
         <v>-54777</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="47">
         <v>-65228</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="110"/>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
-    </row>
-    <row r="18" spans="1:9" s="70" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
+      <c r="G17" s="109"/>
+      <c r="H17" s="106"/>
+      <c r="I17" s="106"/>
+    </row>
+    <row r="18" spans="1:9" s="69" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="47">
         <v>27918</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="47">
         <v>12775</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="47">
         <v>7883</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="110"/>
+      <c r="G18" s="109"/>
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="110"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="109"/>
     </row>
     <row r="20" spans="1:9" s="27" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="46">
+      <c r="B20" s="45">
         <v>-70442</v>
       </c>
-      <c r="C20" s="46">
+      <c r="C20" s="45">
         <v>-67553</v>
       </c>
-      <c r="D20" s="46">
+      <c r="D20" s="45">
         <v>-73111</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="45" t="s">
+      <c r="F20" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="111"/>
+      <c r="G20" s="110"/>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
@@ -3213,136 +3214,136 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="121"/>
-      <c r="F21" s="121"/>
-      <c r="G21" s="110"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
+      <c r="G21" s="109"/>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B22" s="46">
         <v>-197888</v>
       </c>
-      <c r="C22" s="47">
+      <c r="C22" s="46">
         <v>-103420</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="46">
         <v>-83507</v>
       </c>
-      <c r="E22" s="47">
+      <c r="E22" s="46">
         <v>-58519</v>
       </c>
-      <c r="F22" s="47">
+      <c r="F22" s="46">
         <v>-443334</v>
       </c>
-      <c r="G22" s="110"/>
+      <c r="G22" s="109"/>
     </row>
     <row r="23" spans="1:9" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="65">
+      <c r="B23" s="64">
         <v>-10.199999999999999</v>
       </c>
-      <c r="C23" s="65">
+      <c r="C23" s="64">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="D23" s="66">
+      <c r="D23" s="65">
         <v>-4</v>
       </c>
-      <c r="E23" s="66">
+      <c r="E23" s="65">
         <v>-2.7</v>
       </c>
-      <c r="F23" s="66"/>
-      <c r="G23" s="110"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="109"/>
     </row>
     <row r="24" spans="1:9" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="122"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="119"/>
-      <c r="G24" s="110"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="118"/>
+      <c r="G24" s="109"/>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="46">
+      <c r="B25" s="45">
         <v>7818</v>
       </c>
-      <c r="C25" s="116">
+      <c r="C25" s="115">
         <v>9906</v>
       </c>
-      <c r="D25" s="108">
+      <c r="D25" s="107">
         <v>11013</v>
       </c>
-      <c r="E25" s="108">
+      <c r="E25" s="107">
         <v>10819</v>
       </c>
-      <c r="F25" s="108">
+      <c r="F25" s="107">
         <v>39556</v>
       </c>
-      <c r="G25" s="110"/>
+      <c r="G25" s="109"/>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="47">
+      <c r="B26" s="46">
         <v>-205706</v>
       </c>
-      <c r="C26" s="47">
+      <c r="C26" s="46">
         <v>-113326</v>
       </c>
-      <c r="D26" s="90">
+      <c r="D26" s="89">
         <v>-94520</v>
       </c>
-      <c r="E26" s="90">
+      <c r="E26" s="89">
         <v>-69338</v>
       </c>
-      <c r="F26" s="124">
+      <c r="F26" s="123">
         <v>-482890</v>
       </c>
-      <c r="G26" s="110"/>
+      <c r="G26" s="109"/>
     </row>
     <row r="27" spans="1:9" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="65">
+      <c r="B27" s="64">
         <v>-10.6</v>
       </c>
-      <c r="C27" s="65">
+      <c r="C27" s="64">
         <v>-5.6</v>
       </c>
-      <c r="D27" s="66">
+      <c r="D27" s="65">
         <v>-4.5</v>
       </c>
-      <c r="E27" s="66">
+      <c r="E27" s="65">
         <v>-3.1</v>
       </c>
-      <c r="F27" s="123"/>
-      <c r="G27" s="110"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="109"/>
     </row>
     <row r="28" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E28" s="115"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
+      <c r="E28" s="114"/>
+      <c r="F28" s="114"/>
+      <c r="G28" s="114"/>
     </row>
     <row r="29" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E29" s="115"/>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
+      <c r="E29" s="114"/>
+      <c r="F29" s="114"/>
+      <c r="G29" s="114"/>
     </row>
     <row r="30" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E30" s="115"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="115"/>
+      <c r="E30" s="114"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="114"/>
     </row>
     <row r="31" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3351,23 +3352,23 @@
     <row r="35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4E28AB2B-9926-4755-99E6-883815CD2322}" hiddenRows="1">
+    <customSheetView guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}" scale="140" hiddenRows="1">
+      <selection activeCell="A27" sqref="A27"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}" hiddenRows="1">
       <selection activeCell="E7" sqref="E7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{8A1CB61A-793E-4812-8741-E8528853CB5E}" scale="140" hiddenRows="1">
       <selection activeCell="A27" sqref="A27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}" hiddenRows="1">
-      <selection activeCell="E7" sqref="E7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}" scale="140" hiddenRows="1">
-      <selection activeCell="A27" sqref="A27"/>
+    <customSheetView guid="{4E28AB2B-9926-4755-99E6-883815CD2322}" hiddenRows="1">
+      <selection activeCell="E7" sqref="E7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
     </customSheetView>
@@ -3398,273 +3399,273 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
     </row>
     <row r="3" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="126"/>
-      <c r="B3" s="149" t="s">
+      <c r="A3" s="125"/>
+      <c r="B3" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="149"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
     </row>
     <row r="4" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127"/>
-      <c r="B4" s="128" t="s">
+      <c r="A4" s="126"/>
+      <c r="B4" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="129" t="s">
+      <c r="C4" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="129" t="s">
+      <c r="D4" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="129" t="s">
+      <c r="E4" s="128" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="127"/>
-      <c r="B5" s="130" t="s">
+      <c r="A5" s="126"/>
+      <c r="B5" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="131" t="s">
+      <c r="D5" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="131" t="s">
+      <c r="E5" s="130" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="132" t="s">
+      <c r="A6" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="133"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
+      <c r="B6" s="132"/>
+      <c r="C6" s="133"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
     </row>
     <row r="7" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="135" t="s">
+      <c r="A7" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="136">
+      <c r="B7" s="135">
         <v>490.4</v>
       </c>
-      <c r="C7" s="137">
+      <c r="C7" s="136">
         <v>364.8</v>
       </c>
-      <c r="D7" s="137">
+      <c r="D7" s="136">
         <v>365.8</v>
       </c>
-      <c r="E7" s="137">
+      <c r="E7" s="136">
         <v>381.2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="138" t="s">
+      <c r="A8" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="136">
+      <c r="B8" s="135">
         <v>98.4</v>
       </c>
-      <c r="C8" s="137">
+      <c r="C8" s="136">
         <v>95.5</v>
       </c>
-      <c r="D8" s="137">
+      <c r="D8" s="136">
         <v>95.9</v>
       </c>
-      <c r="E8" s="137">
+      <c r="E8" s="136">
         <v>98.1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="139">
+      <c r="B9" s="138">
         <v>588.79999999999995</v>
       </c>
-      <c r="C9" s="140">
+      <c r="C9" s="139">
         <v>460.3</v>
       </c>
-      <c r="D9" s="140">
+      <c r="D9" s="139">
         <v>461.7</v>
       </c>
-      <c r="E9" s="140">
+      <c r="E9" s="139">
         <v>479.3</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="136">
+      <c r="B10" s="135">
         <v>91.1</v>
       </c>
-      <c r="C10" s="137">
+      <c r="C10" s="136">
         <v>88.9</v>
       </c>
-      <c r="D10" s="137">
+      <c r="D10" s="136">
         <v>88.4</v>
       </c>
-      <c r="E10" s="137">
+      <c r="E10" s="136">
         <v>88.9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="127"/>
-      <c r="B11" s="136"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137"/>
+      <c r="A11" s="126"/>
+      <c r="B11" s="135"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
     </row>
     <row r="12" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="132" t="s">
+      <c r="A12" s="131" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="136"/>
-      <c r="C12" s="137"/>
-      <c r="D12" s="137"/>
-      <c r="E12" s="137"/>
+      <c r="B12" s="135"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
     </row>
     <row r="13" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="136">
+      <c r="B13" s="135">
         <v>19.399999999999999</v>
       </c>
-      <c r="C13" s="137">
+      <c r="C13" s="136">
         <v>21.1</v>
       </c>
-      <c r="D13" s="137">
+      <c r="D13" s="136">
         <v>22.3</v>
       </c>
-      <c r="E13" s="137">
+      <c r="E13" s="136">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="138" t="s">
+      <c r="A14" s="137" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="136">
+      <c r="B14" s="135">
         <v>14.4</v>
       </c>
-      <c r="C14" s="137">
+      <c r="C14" s="136">
         <v>16.399999999999999</v>
       </c>
-      <c r="D14" s="137">
+      <c r="D14" s="136">
         <v>15.7</v>
       </c>
-      <c r="E14" s="137">
+      <c r="E14" s="136">
         <v>15.4</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="138" t="s">
+      <c r="A15" s="137" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="136">
+      <c r="B15" s="135">
         <v>23.5</v>
       </c>
-      <c r="C15" s="137">
+      <c r="C15" s="136">
         <v>19.8</v>
       </c>
-      <c r="D15" s="137">
+      <c r="D15" s="136">
         <v>22.5</v>
       </c>
-      <c r="E15" s="137">
+      <c r="E15" s="136">
         <v>20.399999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="132" t="s">
+      <c r="A16" s="131" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="139">
+      <c r="B16" s="138">
         <v>57.3</v>
       </c>
-      <c r="C16" s="140">
+      <c r="C16" s="139">
         <v>57.2</v>
       </c>
-      <c r="D16" s="140">
+      <c r="D16" s="139">
         <v>60.6</v>
       </c>
-      <c r="E16" s="140">
+      <c r="E16" s="139">
         <v>59.8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="127" t="s">
+      <c r="A17" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="136">
+      <c r="B17" s="135">
         <v>8.9</v>
       </c>
-      <c r="C17" s="137">
+      <c r="C17" s="136">
         <v>11.1</v>
       </c>
-      <c r="D17" s="137">
+      <c r="D17" s="136">
         <v>11.6</v>
       </c>
-      <c r="E17" s="137">
+      <c r="E17" s="136">
         <v>11.1</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="127"/>
-      <c r="B18" s="141"/>
-      <c r="C18" s="127"/>
-      <c r="D18" s="127"/>
-      <c r="E18" s="127"/>
+      <c r="A18" s="126"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
     </row>
     <row r="19" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="142" t="s">
+      <c r="A19" s="141" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="139">
+      <c r="B19" s="138">
         <v>646.1</v>
       </c>
-      <c r="C19" s="140">
+      <c r="C19" s="139">
         <v>517.5</v>
       </c>
-      <c r="D19" s="140">
+      <c r="D19" s="139">
         <v>522.29999999999995</v>
       </c>
-      <c r="E19" s="140">
+      <c r="E19" s="139">
         <v>539.1</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4E28AB2B-9926-4755-99E6-883815CD2322}" scale="140">
+    <customSheetView guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}" scale="140">
       <selection activeCell="E5" sqref="E5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{8A1CB61A-793E-4812-8741-E8528853CB5E}" scale="140">
+    <customSheetView guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}" scale="140">
       <selection activeCell="E5" sqref="E5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{344BF70F-4B6B-4B22-B792-A3494CC9D122}" scale="140">
+    <customSheetView guid="{8A1CB61A-793E-4812-8741-E8528853CB5E}" scale="140">
       <selection activeCell="E5" sqref="E5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{15C5EB09-0B76-4C54-83E1-66A9CA1B7502}" scale="140">
+    <customSheetView guid="{4E28AB2B-9926-4755-99E6-883815CD2322}" scale="140">
       <selection activeCell="E5" sqref="E5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
@@ -3679,70 +3680,48 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="0f563589-9cf9-4143-b1eb-fb0534803d38">
+      <Value>183</Value>
+      <Value>6</Value>
+    </TaxCatchAll>
+    <Balance_x0020_sheet_x0020_task_x0020_link xmlns="33ba041c-774b-44c1-b93c-f4d761ad1be8" xsi:nil="true"/>
+    <lb508a4dc5e84436a0fe496b536466aa xmlns="e544e5cc-ab70-42e1-849e-1a0f8bb1f4ef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">TSY RA-8729 - Destroy 10 years after action completed</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">5e6f0879-8127-4ad1-9c47-cf975c4e3f0b</TermId>
+        </TermInfo>
+      </Terms>
+    </lb508a4dc5e84436a0fe496b536466aa>
+    <fd157edda9eb4c38ad6a15be64f62ebc xmlns="33ba041c-774b-44c1-b93c-f4d761ad1be8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">PBO</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">5a7ec2ea-a5be-4656-a359-763d48445a99</TermId>
+        </TermInfo>
+      </Terms>
+    </fd157edda9eb4c38ad6a15be64f62ebc>
+    <Document_x0020_Purpose xmlns="33ba041c-774b-44c1-b93c-f4d761ad1be8">Working document</Document_x0020_Purpose>
+    <Document_x0020_Topic xmlns="33ba041c-774b-44c1-b93c-f4d761ad1be8">Budget process</Document_x0020_Topic>
+    <_dlc_DocId xmlns="0f563589-9cf9-4143-b1eb-fb0534803d38">2020FG-88-8317</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="0f563589-9cf9-4143-b1eb-fb0534803d38">
+      <Url>http://tweb/sites/fg/bpd/_layouts/15/DocIdRedir.aspx?ID=2020FG-88-8317</Url>
+      <Description>2020FG-88-8317</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<p:Policy xmlns:p="office.server.policy" id="" local="true">
-  <p:Name>Treasury Document</p:Name>
-  <p:Description/>
-  <p:Statement/>
-  <p:PolicyItems>
-    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.PolicyAudit" staticId="0x010100348D01E61E107C4DA4B97E380EA20D47|1757814118" UniqueId="2079b4ee-6208-4500-a6e7-1bf5637d01b9">
-      <p:Name>Auditing</p:Name>
-      <p:Description>Audits user actions on documents and list items to the Audit Log.</p:Description>
-      <p:CustomData>
-        <Audit>
-          <Update/>
-          <DeleteRestore/>
-        </Audit>
-      </p:CustomData>
-    </p:PolicyItem>
-  </p:PolicyItems>
-</p:Policy>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4002,61 +3981,95 @@
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:Policy xmlns:p="office.server.policy" id="" local="true">
+  <p:Name>Treasury Document</p:Name>
+  <p:Description/>
+  <p:Statement/>
+  <p:PolicyItems>
+    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.PolicyAudit" staticId="0x010100348D01E61E107C4DA4B97E380EA20D47|1757814118" UniqueId="2079b4ee-6208-4500-a6e7-1bf5637d01b9">
+      <p:Name>Auditing</p:Name>
+      <p:Description>Audits user actions on documents and list items to the Audit Log.</p:Description>
+      <p:CustomData>
+        <Audit>
+          <Update/>
+          <DeleteRestore/>
+        </Audit>
+      </p:CustomData>
+    </p:PolicyItem>
+  </p:PolicyItems>
+</p:Policy>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="0f563589-9cf9-4143-b1eb-fb0534803d38">
-      <Value>183</Value>
-      <Value>6</Value>
-    </TaxCatchAll>
-    <Balance_x0020_sheet_x0020_task_x0020_link xmlns="33ba041c-774b-44c1-b93c-f4d761ad1be8" xsi:nil="true"/>
-    <lb508a4dc5e84436a0fe496b536466aa xmlns="e544e5cc-ab70-42e1-849e-1a0f8bb1f4ef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">TSY RA-8729 - Destroy 10 years after action completed</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">5e6f0879-8127-4ad1-9c47-cf975c4e3f0b</TermId>
-        </TermInfo>
-      </Terms>
-    </lb508a4dc5e84436a0fe496b536466aa>
-    <fd157edda9eb4c38ad6a15be64f62ebc xmlns="33ba041c-774b-44c1-b93c-f4d761ad1be8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">PBO</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">5a7ec2ea-a5be-4656-a359-763d48445a99</TermId>
-        </TermInfo>
-      </Terms>
-    </fd157edda9eb4c38ad6a15be64f62ebc>
-    <Document_x0020_Purpose xmlns="33ba041c-774b-44c1-b93c-f4d761ad1be8">Working document</Document_x0020_Purpose>
-    <Document_x0020_Topic xmlns="33ba041c-774b-44c1-b93c-f4d761ad1be8">Budget process</Document_x0020_Topic>
-    <_dlc_DocId xmlns="0f563589-9cf9-4143-b1eb-fb0534803d38">2020FG-88-8317</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="0f563589-9cf9-4143-b1eb-fb0534803d38">
-      <Url>http://tweb/sites/fg/bpd/_layouts/15/DocIdRedir.aspx?ID=2020FG-88-8317</Url>
-      <Description>2020FG-88-8317</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3479E19-9305-45D9-8F6A-353F5277730B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7042475-4CE8-459B-9167-CBED7CEF5E5D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e544e5cc-ab70-42e1-849e-1a0f8bb1f4ef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="33ba041c-774b-44c1-b93c-f4d761ad1be8"/>
+    <ds:schemaRef ds:uri="0f563589-9cf9-4143-b1eb-fb0534803d38"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76475113-E3EB-489B-9ECE-396C842F2DEA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CDF537D-43FB-4238-AB67-A26FD77A919F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="office.server.policy"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4084,29 +4097,17 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CDF537D-43FB-4238-AB67-A26FD77A919F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76475113-E3EB-489B-9ECE-396C842F2DEA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="office.server.policy"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7042475-4CE8-459B-9167-CBED7CEF5E5D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3479E19-9305-45D9-8F6A-353F5277730B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e544e5cc-ab70-42e1-849e-1a0f8bb1f4ef"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="33ba041c-774b-44c1-b93c-f4d761ad1be8"/>
-    <ds:schemaRef ds:uri="0f563589-9cf9-4143-b1eb-fb0534803d38"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>